<commit_message>
delete content type materiales de estudio
</commit_message>
<xml_diff>
--- a/profiles/andes/modules/custom/udla_load_events/format/eventos.xlsx
+++ b/profiles/andes/modules/custom/udla_load_events/format/eventos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t xml:space="preserve"> title_field_es</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>field_agendar_en</t>
-  </si>
-  <si>
-    <t>Titulo en español</t>
-  </si>
-  <si>
-    <t>Titulo en Ingles</t>
   </si>
   <si>
     <t>Body en español</t>
@@ -134,12 +128,75 @@
    "field_enlace_ver_mas":{"title":"Amazon","url":"https://www.amazon.com"}}
 ]</t>
   </si>
+  <si>
+    <t>Titulo en español2</t>
+  </si>
+  <si>
+    <t>Titulo en español3</t>
+  </si>
+  <si>
+    <t>Titulo en español4</t>
+  </si>
+  <si>
+    <t>Titulo en español5</t>
+  </si>
+  <si>
+    <t>Titulo en español6</t>
+  </si>
+  <si>
+    <t>Titulo en español7</t>
+  </si>
+  <si>
+    <t>Titulo en español8</t>
+  </si>
+  <si>
+    <t>Titulo en español9</t>
+  </si>
+  <si>
+    <t>Titulo en español1</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles1</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles2</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles3</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles4</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles5</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles6</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles7</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles8</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles9</t>
+  </si>
+  <si>
+    <t>Titulo en español10</t>
+  </si>
+  <si>
+    <t>Titulo en Ingles10</t>
+  </si>
+  <si>
+    <t>Categoría evento 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,20 +231,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="6"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -226,21 +269,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,31 +314,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -330,6 +361,10 @@
     <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +386,10 @@
     <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -717,94 +756,517 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="35" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="35" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="35" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="K4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="6">
+    </row>
+    <row r="5" spans="1:15" ht="35" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="35" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="5">
         <v>1</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="35" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="35" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>22</v>
+      <c r="L8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="35" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="35" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="35" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>